<commit_message>
Dream 11 desktop commit new
</commit_message>
<xml_diff>
--- a/Dream 11.xlsx
+++ b/Dream 11.xlsx
@@ -1,21 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17726"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ankit Pancholi\Desktop\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Group A" sheetId="3" r:id="rId1"/>
+    <sheet name="Group B" sheetId="1" r:id="rId2"/>
+    <sheet name="IND-PAK" sheetId="2" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="82">
   <si>
     <t>India</t>
   </si>
@@ -126,12 +122,6 @@
     <t>KDinesh Karthik</t>
   </si>
   <si>
-    <t>??</t>
-  </si>
-  <si>
-    <t>Gud</t>
-  </si>
-  <si>
     <t>New allrounder</t>
   </si>
   <si>
@@ -181,12 +171,108 @@
   </si>
   <si>
     <t>Mohammed Hafeez</t>
+  </si>
+  <si>
+    <t>WK</t>
+  </si>
+  <si>
+    <t>AllRounder</t>
+  </si>
+  <si>
+    <t>Bowler</t>
+  </si>
+  <si>
+    <t>WK+Captain</t>
+  </si>
+  <si>
+    <t>South Africa</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>VC</t>
+  </si>
+  <si>
+    <t>Australia</t>
+  </si>
+  <si>
+    <t>Bangladesh</t>
+  </si>
+  <si>
+    <t>England</t>
+  </si>
+  <si>
+    <t>New Zealand</t>
+  </si>
+  <si>
+    <t>David Warner</t>
+  </si>
+  <si>
+    <t>Steven Smith</t>
+  </si>
+  <si>
+    <t>Mitchell Starc</t>
+  </si>
+  <si>
+    <t>Aaron Finch</t>
+  </si>
+  <si>
+    <t>Glenn Maxwell</t>
+  </si>
+  <si>
+    <t>Marcus Stoinis</t>
+  </si>
+  <si>
+    <t>Chris Lynn</t>
+  </si>
+  <si>
+    <t>Adam Zampa</t>
+  </si>
+  <si>
+    <t>Travis Head</t>
+  </si>
+  <si>
+    <t>Pat Cummins</t>
+  </si>
+  <si>
+    <t>Josh Hazlewood</t>
+  </si>
+  <si>
+    <t>James Pattinson</t>
+  </si>
+  <si>
+    <t>Matthew Wade</t>
+  </si>
+  <si>
+    <t>John Hastings</t>
+  </si>
+  <si>
+    <t>Moises Henriques</t>
+  </si>
+  <si>
+    <t>Shakib Al Hassan</t>
+  </si>
+  <si>
+    <t>Tamim Iqbal</t>
+  </si>
+  <si>
+    <t>Mahmudullah</t>
+  </si>
+  <si>
+    <t>Mustafizur Rahman</t>
+  </si>
+  <si>
+    <t>Soumya Sarkar</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Mushfiqur Rahim</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -541,7 +627,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -549,166 +635,441 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F16"/>
+  <dimension ref="A1:J16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="3.140625" customWidth="1"/>
+    <col min="4" max="4" width="20" customWidth="1"/>
+    <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="3.140625" customWidth="1"/>
+    <col min="7" max="7" width="15.85546875" customWidth="1"/>
+    <col min="9" max="9" width="3.140625" customWidth="1"/>
+    <col min="10" max="10" width="18" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D2" t="s">
+        <v>77</v>
+      </c>
+      <c r="E2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>62</v>
+      </c>
+      <c r="B3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D3" t="s">
+        <v>80</v>
+      </c>
+      <c r="E3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>64</v>
+      </c>
+      <c r="B4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>67</v>
+      </c>
+      <c r="B5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>75</v>
+      </c>
+      <c r="B6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>73</v>
+      </c>
+      <c r="B7" t="s">
+        <v>50</v>
+      </c>
+      <c r="D7" t="s">
+        <v>81</v>
+      </c>
+      <c r="E7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>65</v>
+      </c>
+      <c r="B8" t="s">
+        <v>51</v>
+      </c>
+      <c r="D8" t="s">
+        <v>76</v>
+      </c>
+      <c r="E8" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>66</v>
+      </c>
+      <c r="B9" t="s">
+        <v>51</v>
+      </c>
+      <c r="D9" t="s">
+        <v>78</v>
+      </c>
+      <c r="E9" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>69</v>
+      </c>
+      <c r="B10" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>70</v>
+      </c>
+      <c r="B11" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>63</v>
+      </c>
+      <c r="B12" t="s">
+        <v>52</v>
+      </c>
+      <c r="D12" t="s">
+        <v>79</v>
+      </c>
+      <c r="E12" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>68</v>
+      </c>
+      <c r="B13" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>71</v>
+      </c>
+      <c r="B14" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>72</v>
+      </c>
+      <c r="B15" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>74</v>
+      </c>
+      <c r="B16" t="s">
+        <v>52</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="3.5703125" customWidth="1"/>
+    <col min="4" max="4" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="3.5703125" customWidth="1"/>
+    <col min="7" max="7" width="18.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" s="2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G1" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
-      <c r="C2" t="s">
+      <c r="B2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D2" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>12</v>
       </c>
-      <c r="C3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
-      <c r="C4" t="s">
-        <v>18</v>
+      <c r="B4" t="s">
+        <v>31</v>
       </c>
       <c r="D4" t="s">
-        <v>31</v>
-      </c>
-      <c r="F4" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+      <c r="E4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>14</v>
       </c>
-      <c r="C5" t="s">
-        <v>19</v>
+      <c r="B5" t="s">
+        <v>31</v>
       </c>
       <c r="D5" t="s">
-        <v>31</v>
-      </c>
-      <c r="E5">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+      <c r="E5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>11</v>
       </c>
-      <c r="C6" t="s">
-        <v>20</v>
-      </c>
-      <c r="D6" t="s">
-        <v>35</v>
-      </c>
-      <c r="E6">
-        <v>7.5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>31</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E6" t="s">
+        <v>31</v>
+      </c>
+      <c r="G6" s="1"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>31</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E7" t="s">
+        <v>31</v>
+      </c>
+      <c r="G7" s="1"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>50</v>
+      </c>
+      <c r="D8" t="s">
+        <v>23</v>
+      </c>
+      <c r="E8" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>32</v>
       </c>
-      <c r="C9" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>50</v>
+      </c>
+      <c r="D9" t="s">
+        <v>29</v>
+      </c>
+      <c r="E9" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>10</v>
       </c>
       <c r="B10" t="s">
+        <v>51</v>
+      </c>
+      <c r="D10" t="s">
+        <v>27</v>
+      </c>
+      <c r="E10" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>6</v>
+      </c>
+      <c r="B11" t="s">
+        <v>51</v>
+      </c>
+      <c r="D11" t="s">
+        <v>24</v>
+      </c>
+      <c r="E11" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>2</v>
+      </c>
+      <c r="B12" t="s">
+        <v>52</v>
+      </c>
+      <c r="D12" t="s">
+        <v>20</v>
+      </c>
+      <c r="E12" t="s">
         <v>33</v>
       </c>
-      <c r="C10" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="B13" t="s">
+        <v>52</v>
+      </c>
+      <c r="D13" s="1" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+      <c r="E13" t="s">
+        <v>52</v>
+      </c>
+      <c r="G13" s="1"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>9</v>
       </c>
-      <c r="C12" t="s">
+      <c r="B14" t="s">
+        <v>52</v>
+      </c>
+      <c r="D14" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>6</v>
-      </c>
-      <c r="C13" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+      <c r="E14" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>13</v>
       </c>
-      <c r="C14" t="s">
+      <c r="B15" t="s">
+        <v>52</v>
+      </c>
+      <c r="D15" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>2</v>
-      </c>
-      <c r="C15" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E15" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>3</v>
       </c>
-      <c r="C16" t="s">
+      <c r="B16" t="s">
+        <v>52</v>
+      </c>
+      <c r="D16" t="s">
         <v>30</v>
+      </c>
+      <c r="E16" t="s">
+        <v>52</v>
       </c>
     </row>
   </sheetData>
@@ -717,11 +1078,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H12"/>
+  <dimension ref="A1:I12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -730,235 +1093,253 @@
     <col min="7" max="7" width="19.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="D1" s="2" t="s">
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>37</v>
       </c>
-      <c r="G1" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>39</v>
-      </c>
       <c r="B2" t="s">
-        <v>49</v>
+        <v>47</v>
+      </c>
+      <c r="C2" t="s">
+        <v>55</v>
       </c>
       <c r="D2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E2" t="s">
-        <v>49</v>
+        <v>47</v>
+      </c>
+      <c r="F2" t="s">
+        <v>55</v>
       </c>
       <c r="G2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="H2" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+        <v>47</v>
+      </c>
+      <c r="I2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>19</v>
       </c>
       <c r="B3" t="s">
-        <v>50</v>
+        <v>48</v>
+      </c>
+      <c r="C3" t="s">
+        <v>56</v>
       </c>
       <c r="D3" t="s">
         <v>19</v>
       </c>
       <c r="E3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="G3" t="s">
         <v>19</v>
       </c>
       <c r="H3" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B4" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D4" t="s">
         <v>18</v>
       </c>
       <c r="E4" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="G4" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="H4" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>14</v>
       </c>
       <c r="B5" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D5" t="s">
         <v>29</v>
       </c>
       <c r="E5" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="G5" t="s">
+        <v>46</v>
+      </c>
+      <c r="H5" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>40</v>
+      </c>
+      <c r="B6" t="s">
+        <v>47</v>
+      </c>
+      <c r="D6" t="s">
+        <v>44</v>
+      </c>
+      <c r="E6" t="s">
         <v>48</v>
-      </c>
-      <c r="H5" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>42</v>
-      </c>
-      <c r="B6" t="s">
-        <v>49</v>
-      </c>
-      <c r="D6" t="s">
-        <v>46</v>
-      </c>
-      <c r="E6" t="s">
-        <v>50</v>
       </c>
       <c r="G6" t="s">
         <v>29</v>
       </c>
       <c r="H6" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+        <v>48</v>
+      </c>
+      <c r="I6" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B7" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D7" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E7" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="G7" t="s">
         <v>18</v>
       </c>
       <c r="H7" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B8" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D8" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E8" t="s">
-        <v>49</v>
+        <v>47</v>
+      </c>
+      <c r="F8" t="s">
+        <v>56</v>
       </c>
       <c r="G8" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="H8" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B9" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D9" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E9" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="G9" t="s">
         <v>20</v>
       </c>
       <c r="H9" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>23</v>
       </c>
       <c r="B10" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D10" t="s">
         <v>30</v>
       </c>
       <c r="E10" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="G10" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="H10" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B11" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D11" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E11" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="G11" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="H11" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>30</v>
       </c>
       <c r="B12" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D12" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E12" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="G12" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="H12" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Dream 11 desktop commit Aus-Ban
</commit_message>
<xml_diff>
--- a/Dream 11.xlsx
+++ b/Dream 11.xlsx
@@ -4,12 +4,13 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Group A" sheetId="3" r:id="rId1"/>
     <sheet name="Group B" sheetId="1" r:id="rId2"/>
     <sheet name="IND-PAK" sheetId="2" r:id="rId3"/>
+    <sheet name="Aus-Ban" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="145621"/>
   <extLst>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="100">
   <si>
     <t>India</t>
   </si>
@@ -83,9 +84,6 @@
     <t>Babar Azam</t>
   </si>
   <si>
-    <t>Fahim Ashraf</t>
-  </si>
-  <si>
     <t>Fakhar Zaman</t>
   </si>
   <si>
@@ -266,14 +264,71 @@
     <t>Soumya Sarkar</t>
   </si>
   <si>
-    <t xml:space="preserve"> Mushfiqur Rahim</t>
+    <t>Mushfiqur Rahim</t>
+  </si>
+  <si>
+    <t>Mashrafe Mortaza</t>
+  </si>
+  <si>
+    <t>Taskin Ahmed</t>
+  </si>
+  <si>
+    <t>Sabbir-Rahman</t>
+  </si>
+  <si>
+    <t>Shafiul Islam</t>
+  </si>
+  <si>
+    <t>Mehedi Hasan</t>
+  </si>
+  <si>
+    <t>Rubel Hossain</t>
+  </si>
+  <si>
+    <t>Mosaddek Hossain</t>
+  </si>
+  <si>
+    <t>Imrul Kayes</t>
+  </si>
+  <si>
+    <t>Sunzamul Islam</t>
+  </si>
+  <si>
+    <t>Faheem Ashraf</t>
+  </si>
+  <si>
+    <t>SriLanka</t>
+  </si>
+  <si>
+    <t>AUS</t>
+  </si>
+  <si>
+    <t>BAN</t>
+  </si>
+  <si>
+    <t>Earned</t>
+  </si>
+  <si>
+    <t>P/L</t>
+  </si>
+  <si>
+    <t>Invested</t>
+  </si>
+  <si>
+    <t>Captain</t>
+  </si>
+  <si>
+    <t>Vice-Captain</t>
+  </si>
+  <si>
+    <t>Allrounder</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -296,16 +351,42 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -313,20 +394,47 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FF20CF17"/>
+      <color rgb="FF00BC00"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -637,98 +745,116 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A11" sqref="A11:B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="3.140625" customWidth="1"/>
+    <col min="3" max="3" width="4.7109375" customWidth="1"/>
     <col min="4" max="4" width="20" customWidth="1"/>
     <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="3.140625" customWidth="1"/>
+    <col min="6" max="6" width="4.42578125" customWidth="1"/>
     <col min="7" max="7" width="15.85546875" customWidth="1"/>
-    <col min="9" max="9" width="3.140625" customWidth="1"/>
+    <col min="9" max="9" width="4.42578125" customWidth="1"/>
     <col min="10" max="10" width="18" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>59</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B4" t="s">
-        <v>31</v>
+        <v>30</v>
+      </c>
+      <c r="D4" t="s">
+        <v>83</v>
+      </c>
+      <c r="E4" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B5" t="s">
-        <v>31</v>
+        <v>30</v>
+      </c>
+      <c r="D5" t="s">
+        <v>88</v>
+      </c>
+      <c r="E5" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B6" t="s">
-        <v>31</v>
+        <v>30</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="E6" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B7" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D7" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="E7" t="s">
         <v>50</v>
@@ -736,92 +862,128 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D8" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="E8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B9" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D9" t="s">
-        <v>78</v>
+        <v>87</v>
       </c>
       <c r="E9" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B10" t="s">
+        <v>50</v>
+      </c>
+      <c r="D10" t="s">
+        <v>78</v>
+      </c>
+      <c r="E10" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B11" t="s">
-        <v>52</v>
+        <v>51</v>
+      </c>
+      <c r="D11" t="s">
+        <v>82</v>
+      </c>
+      <c r="E11" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B12" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D12" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="E12" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B13" t="s">
-        <v>52</v>
+        <v>51</v>
+      </c>
+      <c r="D13" t="s">
+        <v>84</v>
+      </c>
+      <c r="E13" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B14" t="s">
-        <v>52</v>
+        <v>51</v>
+      </c>
+      <c r="D14" t="s">
+        <v>85</v>
+      </c>
+      <c r="E14" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B15" t="s">
-        <v>52</v>
+        <v>51</v>
+      </c>
+      <c r="D15" t="s">
+        <v>86</v>
+      </c>
+      <c r="E15" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B16" t="s">
-        <v>52</v>
+        <v>51</v>
+      </c>
+      <c r="D16" t="s">
+        <v>89</v>
+      </c>
+      <c r="E16" t="s">
+        <v>51</v>
       </c>
     </row>
   </sheetData>
@@ -831,24 +993,23 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G16"/>
+  <dimension ref="A1:J16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="3.5703125" customWidth="1"/>
+    <col min="3" max="3" width="4.42578125" customWidth="1"/>
     <col min="4" max="4" width="18.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="3.5703125" customWidth="1"/>
+    <col min="6" max="6" width="4.42578125" customWidth="1"/>
     <col min="7" max="7" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="4.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -856,220 +1017,223 @@
         <v>15</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+        <v>53</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D2" t="s">
         <v>16</v>
       </c>
       <c r="E2" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>12</v>
       </c>
       <c r="B3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D3" t="s">
         <v>19</v>
       </c>
       <c r="E3" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D4" t="s">
         <v>17</v>
       </c>
       <c r="E4" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>14</v>
       </c>
       <c r="B5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D5" t="s">
         <v>18</v>
       </c>
       <c r="E5" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>11</v>
       </c>
       <c r="B6" t="s">
-        <v>31</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>21</v>
+        <v>30</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>20</v>
       </c>
       <c r="E6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G6" s="1"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>31</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>22</v>
+        <v>30</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>21</v>
       </c>
       <c r="E7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G7" s="1"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>5</v>
       </c>
       <c r="B8" t="s">
+        <v>49</v>
+      </c>
+      <c r="D8" t="s">
+        <v>22</v>
+      </c>
+      <c r="E8" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>31</v>
+      </c>
+      <c r="B9" t="s">
+        <v>49</v>
+      </c>
+      <c r="D9" t="s">
+        <v>28</v>
+      </c>
+      <c r="E9" t="s">
         <v>50</v>
       </c>
-      <c r="D8" t="s">
-        <v>23</v>
-      </c>
-      <c r="E8" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>32</v>
-      </c>
-      <c r="B9" t="s">
-        <v>50</v>
-      </c>
-      <c r="D9" t="s">
-        <v>29</v>
-      </c>
-      <c r="E9" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>10</v>
       </c>
       <c r="B10" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D10" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E10" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>6</v>
       </c>
       <c r="B11" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D11" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E11" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>2</v>
       </c>
       <c r="B12" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D12" t="s">
-        <v>20</v>
+        <v>90</v>
       </c>
       <c r="E12" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>8</v>
       </c>
       <c r="B13" t="s">
-        <v>52</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>25</v>
+        <v>51</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>24</v>
       </c>
       <c r="E13" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G13" s="1"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>9</v>
       </c>
       <c r="B14" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D14" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E14" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D15" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E15" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>3</v>
       </c>
       <c r="B16" t="s">
-        <v>52</v>
-      </c>
-      <c r="D16" t="s">
-        <v>30</v>
+        <v>51</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>29</v>
       </c>
       <c r="E16" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
   </sheetData>
@@ -1080,10 +1244,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I12"/>
+  <dimension ref="A1:I16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1095,42 +1259,42 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>35</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="I2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -1138,42 +1302,42 @@
         <v>19</v>
       </c>
       <c r="B3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D3" t="s">
         <v>19</v>
       </c>
       <c r="E3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G3" t="s">
         <v>19</v>
       </c>
       <c r="H3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D4" t="s">
         <v>18</v>
       </c>
       <c r="E4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -1181,165 +1345,548 @@
         <v>14</v>
       </c>
       <c r="B5" t="s">
+        <v>46</v>
+      </c>
+      <c r="D5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E5" t="s">
         <v>47</v>
       </c>
-      <c r="D5" t="s">
-        <v>29</v>
-      </c>
-      <c r="E5" t="s">
-        <v>48</v>
-      </c>
       <c r="G5" t="s">
+        <v>45</v>
+      </c>
+      <c r="H5" t="s">
         <v>46</v>
-      </c>
-      <c r="H5" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B6" t="s">
+        <v>46</v>
+      </c>
+      <c r="D6" t="s">
+        <v>43</v>
+      </c>
+      <c r="E6" t="s">
         <v>47</v>
       </c>
-      <c r="D6" t="s">
-        <v>44</v>
-      </c>
-      <c r="E6" t="s">
-        <v>48</v>
-      </c>
       <c r="G6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="I6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G7" t="s">
         <v>18</v>
       </c>
       <c r="H7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B9" t="s">
+        <v>46</v>
+      </c>
+      <c r="D9" t="s">
+        <v>40</v>
+      </c>
+      <c r="E9" t="s">
+        <v>46</v>
+      </c>
+      <c r="G9" t="s">
+        <v>90</v>
+      </c>
+      <c r="H9" t="s">
         <v>47</v>
-      </c>
-      <c r="D9" t="s">
-        <v>41</v>
-      </c>
-      <c r="E9" t="s">
-        <v>47</v>
-      </c>
-      <c r="G9" t="s">
-        <v>20</v>
-      </c>
-      <c r="H9" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H10" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>40</v>
+      </c>
+      <c r="B11" t="s">
+        <v>46</v>
+      </c>
+      <c r="D11" t="s">
         <v>41</v>
       </c>
-      <c r="B11" t="s">
+      <c r="E11" t="s">
         <v>47</v>
       </c>
-      <c r="D11" t="s">
-        <v>42</v>
-      </c>
-      <c r="E11" t="s">
-        <v>48</v>
-      </c>
       <c r="G11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H11" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B12" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D12" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E12" t="s">
+        <v>46</v>
+      </c>
+      <c r="G12" t="s">
+        <v>41</v>
+      </c>
+      <c r="H12" t="s">
         <v>47</v>
       </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="B14" s="6">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="B15" s="6"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="B16" s="6"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I4" sqref="I4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.85546875" customWidth="1"/>
+    <col min="6" max="6" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2" t="s">
+        <v>92</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="F2" t="s">
+        <v>30</v>
+      </c>
+      <c r="G2" t="s">
+        <v>92</v>
+      </c>
+      <c r="I2" t="s">
+        <v>61</v>
+      </c>
+      <c r="J2" t="s">
+        <v>30</v>
+      </c>
+      <c r="K2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="B3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C3" t="s">
+        <v>92</v>
+      </c>
+      <c r="E3" t="s">
+        <v>61</v>
+      </c>
+      <c r="F3" t="s">
+        <v>30</v>
+      </c>
+      <c r="G3" t="s">
+        <v>92</v>
+      </c>
+      <c r="I3" t="s">
+        <v>79</v>
+      </c>
+      <c r="J3" t="s">
+        <v>30</v>
+      </c>
+      <c r="K3" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>74</v>
+      </c>
+      <c r="B4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C4" t="s">
+        <v>92</v>
+      </c>
+      <c r="E4" t="s">
+        <v>76</v>
+      </c>
+      <c r="F4" t="s">
+        <v>30</v>
+      </c>
+      <c r="G4" t="s">
+        <v>93</v>
+      </c>
+      <c r="I4" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="J4" t="s">
+        <v>30</v>
+      </c>
+      <c r="K4" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>76</v>
+      </c>
+      <c r="B5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C5" t="s">
+        <v>93</v>
+      </c>
+      <c r="E5" t="s">
+        <v>83</v>
+      </c>
+      <c r="F5" t="s">
+        <v>30</v>
+      </c>
+      <c r="G5" t="s">
+        <v>93</v>
+      </c>
+      <c r="I5" t="s">
+        <v>80</v>
+      </c>
+      <c r="J5" t="s">
+        <v>49</v>
+      </c>
+      <c r="K5" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>80</v>
+      </c>
+      <c r="B6" t="s">
+        <v>49</v>
+      </c>
+      <c r="C6" t="s">
+        <v>93</v>
+      </c>
+      <c r="E6" t="s">
+        <v>72</v>
+      </c>
+      <c r="F6" t="s">
+        <v>49</v>
+      </c>
+      <c r="G6" t="s">
+        <v>92</v>
+      </c>
+      <c r="I6" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="J6" t="s">
+        <v>99</v>
+      </c>
+      <c r="K6" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>64</v>
+      </c>
+      <c r="B7" t="s">
+        <v>99</v>
+      </c>
+      <c r="C7" t="s">
+        <v>92</v>
+      </c>
+      <c r="E7" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="F7" t="s">
+        <v>99</v>
+      </c>
+      <c r="G7" t="s">
+        <v>92</v>
+      </c>
+      <c r="I7" t="s">
+        <v>64</v>
+      </c>
+      <c r="J7" t="s">
+        <v>99</v>
+      </c>
+      <c r="K7" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="B8" t="s">
+        <v>99</v>
+      </c>
+      <c r="C8" t="s">
+        <v>93</v>
+      </c>
+      <c r="E8" t="s">
+        <v>75</v>
+      </c>
+      <c r="F8" t="s">
+        <v>99</v>
+      </c>
+      <c r="G8" t="s">
+        <v>93</v>
+      </c>
+      <c r="I8" t="s">
+        <v>68</v>
+      </c>
+      <c r="J8" t="s">
+        <v>50</v>
+      </c>
+      <c r="K8" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>77</v>
+      </c>
+      <c r="B9" t="s">
+        <v>99</v>
+      </c>
+      <c r="C9" t="s">
+        <v>93</v>
+      </c>
+      <c r="E9" t="s">
+        <v>77</v>
+      </c>
+      <c r="F9" t="s">
+        <v>99</v>
+      </c>
+      <c r="G9" t="s">
+        <v>93</v>
+      </c>
+      <c r="I9" t="s">
+        <v>69</v>
+      </c>
+      <c r="J9" t="s">
+        <v>51</v>
+      </c>
+      <c r="K9" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>70</v>
+      </c>
+      <c r="B10" t="s">
+        <v>51</v>
+      </c>
+      <c r="C10" t="s">
+        <v>92</v>
+      </c>
+      <c r="E10" t="s">
+        <v>70</v>
+      </c>
+      <c r="F10" t="s">
+        <v>51</v>
+      </c>
+      <c r="G10" t="s">
+        <v>92</v>
+      </c>
+      <c r="I10" t="s">
+        <v>78</v>
+      </c>
+      <c r="J10" t="s">
+        <v>51</v>
+      </c>
+      <c r="K10" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>73</v>
+      </c>
+      <c r="B11" t="s">
+        <v>51</v>
+      </c>
+      <c r="C11" t="s">
+        <v>92</v>
+      </c>
+      <c r="E11" t="s">
+        <v>62</v>
+      </c>
+      <c r="F11" t="s">
+        <v>51</v>
+      </c>
+      <c r="G11" t="s">
+        <v>92</v>
+      </c>
+      <c r="I11" t="s">
+        <v>62</v>
+      </c>
+      <c r="J11" t="s">
+        <v>51</v>
+      </c>
+      <c r="K11" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>78</v>
+      </c>
+      <c r="B12" t="s">
+        <v>51</v>
+      </c>
+      <c r="C12" t="s">
+        <v>93</v>
+      </c>
+      <c r="E12" t="s">
+        <v>81</v>
+      </c>
+      <c r="F12" t="s">
+        <v>51</v>
+      </c>
       <c r="G12" t="s">
-        <v>42</v>
-      </c>
-      <c r="H12" t="s">
-        <v>48</v>
+        <v>93</v>
+      </c>
+      <c r="I12" t="s">
+        <v>81</v>
+      </c>
+      <c r="J12" t="s">
+        <v>51</v>
+      </c>
+      <c r="K12" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" s="7" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" s="8" t="s">
+        <v>98</v>
       </c>
     </row>
   </sheetData>

</xml_diff>